<commit_message>
wrong file committed before
</commit_message>
<xml_diff>
--- a/FunctionalRequirements.xlsx
+++ b/FunctionalRequirements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>Number</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Interface that allows user to select media, by type or by date</t>
-  </si>
-  <si>
     <t>Unplanned</t>
   </si>
   <si>
@@ -57,19 +54,94 @@
     <t>Interface that allows user to manage profile, passwords, information</t>
   </si>
   <si>
-    <t>Functional Requirements</t>
-  </si>
-  <si>
     <t>Server needs:  Linux server, also availability to run on a rasberry pi</t>
   </si>
   <si>
     <t>Libraries need to be built out for android (Objects that help protect against data intrusion)</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Libraries need to be built out for iOS (objects that help protect against data intrusion)</t>
+  </si>
+  <si>
+    <t>Add Media on website</t>
+  </si>
+  <si>
+    <t>2.1.1</t>
+  </si>
+  <si>
+    <t>Uploader for files, all types</t>
+  </si>
+  <si>
+    <t>2.1.2</t>
+  </si>
+  <si>
+    <t>Uploader to allow message to be entered like a text or tweet</t>
+  </si>
+  <si>
+    <t>Add Media via mobile device</t>
+  </si>
+  <si>
+    <t>Use phone technology to take or upload photo</t>
+  </si>
+  <si>
+    <t>Use phone technology to take or upload video</t>
+  </si>
+  <si>
+    <t>Use phone technology to take or upload vocal message</t>
+  </si>
+  <si>
+    <t>Use phone technology to enter message like text or tweet as well as upload text</t>
+  </si>
+  <si>
+    <t>2.2.1</t>
+  </si>
+  <si>
+    <t>2.2.2</t>
+  </si>
+  <si>
+    <t>2.2.3</t>
+  </si>
+  <si>
+    <t>2.2.4</t>
+  </si>
+  <si>
+    <t>Functional and Non-Functional Requirements</t>
+  </si>
+  <si>
+    <t>Interface that allows user to signup for service</t>
+  </si>
+  <si>
+    <t>Interface that allows user to view media, by type or by date from database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Server software is to be written using PHP </t>
+  </si>
+  <si>
+    <t>Libraries are to be written using java (or until further notice)</t>
+  </si>
+  <si>
+    <t>Libraries need to be written using Objective C (or until further notice)</t>
+  </si>
+  <si>
+    <t>This prototype will give a look and feel for the mobile app and will be the model for the native application</t>
+  </si>
+  <si>
+    <t>If a native application is out side of the scope near the project end date, then prototype will be Evaluated</t>
+  </si>
+  <si>
+    <t>A prototype will be written using a Web application wrapped with each respected application wrapper</t>
+  </si>
+  <si>
+    <t>Data passed to the server will be encrypted</t>
+  </si>
+  <si>
+    <t>Data will be assigned a unique ID, based off the contents of the data and the iterative id of the server</t>
+  </si>
+  <si>
+    <t>passwords will only be able to be matched, no missing password retreival method, only password resets</t>
+  </si>
+  <si>
+    <t>Implementation of Oauth or other type of one type logins will be investigated</t>
   </si>
 </sst>
 </file>
@@ -116,7 +188,9 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,12 +506,12 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -452,123 +526,328 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>4</v>
       </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>5</v>
+      </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>3</v>
+      <c r="A20" s="2">
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>4</v>
-      </c>
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
+      <c r="A21" s="2"/>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>5</v>
+      <c r="A22" s="2">
+        <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
       </c>
       <c r="C23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>11</v>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1</v>
+      <c r="A26" s="2">
+        <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>2</v>
+      <c r="A27" s="2">
+        <v>6</v>
       </c>
       <c r="B27" t="s">
         <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>3</v>
+      <c r="A28" s="2">
+        <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>4</v>
+      <c r="A29" s="2">
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>9</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>12</v>
+      </c>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>13</v>
+      </c>
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>